<commit_message>
added necessary dependency files and short clip
</commit_message>
<xml_diff>
--- a/Data/anonymized_consolidated_purchases.xlsx
+++ b/Data/anonymized_consolidated_purchases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Particulars</t>
   </si>
@@ -22,58 +22,25 @@
     <t>Credit</t>
   </si>
   <si>
-    <t>Achija Chemicals</t>
-  </si>
-  <si>
-    <t>ANBU SALT</t>
-  </si>
-  <si>
-    <t>Cona Chemicals PVT Ltd</t>
-  </si>
-  <si>
-    <t>HK Chems and Dyes</t>
-  </si>
-  <si>
-    <t>Jayvignesh Chemicals</t>
-  </si>
-  <si>
-    <t>KONVIO RO SUSTEM</t>
-  </si>
-  <si>
-    <t>Lalith Chemicals</t>
-  </si>
-  <si>
-    <t>Lok International</t>
-  </si>
-  <si>
-    <t>Mahalakshmi Enterprises</t>
-  </si>
-  <si>
-    <t>Microgeneix Specialities Pvt Ltd</t>
-  </si>
-  <si>
-    <t>NATHAN SALT COMPANY</t>
-  </si>
-  <si>
-    <t>Pawar Chemicals</t>
-  </si>
-  <si>
-    <t>Rajalakshmi Plastic and Chemicals</t>
-  </si>
-  <si>
-    <t>Sabhya Chem</t>
-  </si>
-  <si>
-    <t>Shahi Exports Pvt Ltd</t>
-  </si>
-  <si>
-    <t>Sri Vinayaka Enterprises</t>
-  </si>
-  <si>
-    <t>Supriya Chemicals</t>
-  </si>
-  <si>
-    <t>Synbus INC</t>
+    <t>Polymers</t>
+  </si>
+  <si>
+    <t>Basic Chemicals</t>
+  </si>
+  <si>
+    <t>Cosmetic Chemicals</t>
+  </si>
+  <si>
+    <t>Specialty Chemicals</t>
+  </si>
+  <si>
+    <t>Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Pesticides</t>
+  </si>
+  <si>
+    <t>Biochemicals</t>
   </si>
 </sst>
 </file>
@@ -471,7 +438,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1196479.977023774</v>
@@ -479,7 +446,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>788159.2011586198</v>
@@ -487,7 +454,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>559220.2919883109</v>
@@ -495,7 +462,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>739300.6898017019</v>
@@ -503,7 +470,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>463371.0800198584</v>
@@ -511,7 +478,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>891892.8219590759</v>
@@ -519,7 +486,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>1078350.098877882</v>
@@ -527,7 +494,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>727250.1533629631</v>
@@ -535,7 +502,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>1002669.175419676</v>
@@ -543,7 +510,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>732536.0794357714</v>
@@ -551,7 +518,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>811401.1390137251</v>
@@ -559,7 +526,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>808394.2725760236</v>
@@ -567,7 +534,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>597167.4207140697</v>
@@ -575,7 +542,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B18">
         <v>1082410.501634112</v>
@@ -583,7 +550,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>518269.2876833653</v>

</xml_diff>